<commit_message>
address.ToString(R1C1) now returns R1C1 notation instead of "1,1" Removed methods range.ToStringFixed and range.ToStringRelative. Fixed issues: 6948,6961,6947,6872,6939,6932
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -39,12 +39,18 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="2">
+  <x:fills count="3">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
     <x:fill>
       <x:patternFill patternType="gray125"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF9ACD32"/>
+        <x:bgColor rgb="FF9ACD32"/>
+      </x:patternFill>
     </x:fill>
   </x:fills>
   <x:borders count="1">
@@ -66,13 +72,20 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="1">
+  <x:cellStyleXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="1">
+  <x:cellXfs count="2">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="0" applyFill="1" applyBorder="0" applyAlignment="0" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -376,26 +389,23 @@
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
       <x:c r="C1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3">
-      <x:c r="B2" s="0" t="s"/>
       <x:c r="C2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:3">
-      <x:c r="B3" s="0" t="s"/>
-    </x:row>
     <x:row r="4" spans="1:3">
       <x:c r="A4" s="0" t="s"/>
-      <x:c r="B4" s="0" t="s"/>
     </x:row>
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s"/>
@@ -418,7 +428,7 @@
       <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1 B2:B2">
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -447,80 +457,103 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:E14"/>
+  <x:dimension ref="A1:G14"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:5">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:5">
-      <x:c r="A2" s="0" t="s"/>
-      <x:c r="B2" s="0" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="B4" s="0" t="s"/>
-      <x:c r="C4" s="0" t="s"/>
-      <x:c r="D4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="B5" s="0" t="s"/>
-      <x:c r="C5" s="0" t="s"/>
-      <x:c r="D5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:5">
-      <x:c r="B6" s="0" t="s"/>
-      <x:c r="C6" s="0" t="s"/>
-      <x:c r="D6" s="0" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:5">
-      <x:c r="B7" s="0" t="s"/>
-      <x:c r="C7" s="0" t="s"/>
-      <x:c r="D7" s="0" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:5">
-      <x:c r="A11" s="0" t="s"/>
-      <x:c r="B11" s="0" t="s"/>
-      <x:c r="C11" s="0" t="s"/>
-      <x:c r="D11" s="0" t="s"/>
-      <x:c r="E11" s="0" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:5">
-      <x:c r="A12" s="0" t="s"/>
-      <x:c r="B12" s="0" t="s"/>
-      <x:c r="C12" s="0" t="s"/>
-      <x:c r="D12" s="0" t="s"/>
-      <x:c r="E12" s="0" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:5">
-      <x:c r="A13" s="0" t="s"/>
-      <x:c r="B13" s="0" t="s"/>
-      <x:c r="C13" s="0" t="s"/>
-      <x:c r="D13" s="0" t="s"/>
-      <x:c r="E13" s="0" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:5">
-      <x:c r="A14" s="0" t="s"/>
-      <x:c r="B14" s="0" t="s"/>
-      <x:c r="C14" s="0" t="s"/>
-      <x:c r="D14" s="0" t="s"/>
-      <x:c r="E14" s="0" t="s"/>
+    <x:row r="1" spans="1:7">
+      <x:c r="A1" s="1" t="s"/>
+      <x:c r="B1" s="1" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="1" t="s"/>
+      <x:c r="B2" s="1" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="B4" s="1" t="s"/>
+      <x:c r="C4" s="1" t="s"/>
+      <x:c r="D4" s="1" t="s"/>
+      <x:c r="F4" s="1" t="s"/>
+      <x:c r="G4" s="1" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="B5" s="1" t="s"/>
+      <x:c r="C5" s="1" t="s"/>
+      <x:c r="D5" s="1" t="s"/>
+      <x:c r="F5" s="1" t="s"/>
+      <x:c r="G5" s="1" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="B6" s="1" t="s"/>
+      <x:c r="C6" s="1" t="s"/>
+      <x:c r="D6" s="1" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="B7" s="1" t="s"/>
+      <x:c r="C7" s="1" t="s"/>
+      <x:c r="D7" s="1" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="1" t="s"/>
+      <x:c r="B11" s="1" t="s"/>
+      <x:c r="C11" s="1" t="s"/>
+      <x:c r="D11" s="1" t="s"/>
+      <x:c r="E11" s="1" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="1" t="s"/>
+      <x:c r="B12" s="1" t="s"/>
+      <x:c r="C12" s="1" t="s"/>
+      <x:c r="D12" s="1" t="s"/>
+      <x:c r="E12" s="1" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="A13" s="1" t="s"/>
+      <x:c r="B13" s="1" t="s"/>
+      <x:c r="C13" s="1" t="s"/>
+      <x:c r="D13" s="1" t="s"/>
+      <x:c r="E13" s="1" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="A14" s="1" t="s"/>
+      <x:c r="B14" s="1" t="s"/>
+      <x:c r="C14" s="1" t="s"/>
+      <x:c r="D14" s="1" t="s"/>
+      <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="3">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:G5 A1:A1 B1:B1 A2:A2 C4:C4 D4:D4 C5:C5 D5:D5 C6:C6 D6:D6 C7:C7 D7:D7">
+  <x:dataValidations count="7">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2 B1:B1 C4:C7 D4:D4 D7:D7 F4:F5">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11 C11:C11 D11:D11 E11:E11 A12:A12 C12:C12 D12:D12 E12:E12 A13:A13 B13:B13 C13:C13 D13:D13 E13:E13 A14:A14 B14:B14 C14:C14 D14:D14 E14:E14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 B13:B14 E11:E14 C11:C12 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Fixed memory leak issue
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -8,6 +8,8 @@
   <x:sheets>
     <x:sheet name="Data Validation" sheetId="2" r:id="rId2"/>
     <x:sheet name="Validate Ranges" sheetId="3" r:id="rId3"/>
+    <x:sheet name="Data Validation - Copy" sheetId="4" r:id="rId4"/>
+    <x:sheet name="Validate Ranges - Copy" sheetId="5" r:id="rId5"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -525,19 +527,7 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -583,6 +573,233 @@
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+  </x:dataValidations>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C5"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="0" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s"/>
+      <x:c r="C1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="C2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:dataValidations count="6">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2>5</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
+      <x:formula1>36526</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
+      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+  </x:dataValidations>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:G14"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="0" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:cols>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:7">
+      <x:c r="A1" s="1" t="s"/>
+      <x:c r="B1" s="1" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="1" t="s"/>
+      <x:c r="B2" s="1" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="B4" s="1" t="s"/>
+      <x:c r="C4" s="1" t="s"/>
+      <x:c r="D4" s="1" t="s"/>
+      <x:c r="F4" s="1" t="s"/>
+      <x:c r="G4" s="1" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="B5" s="1" t="s"/>
+      <x:c r="C5" s="1" t="s"/>
+      <x:c r="D5" s="1" t="s"/>
+      <x:c r="F5" s="1" t="s"/>
+      <x:c r="G5" s="1" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="B6" s="1" t="s"/>
+      <x:c r="C6" s="1" t="s"/>
+      <x:c r="D6" s="1" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="B7" s="1" t="s"/>
+      <x:c r="C7" s="1" t="s"/>
+      <x:c r="D7" s="1" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="1" t="s"/>
+      <x:c r="B11" s="1" t="s"/>
+      <x:c r="C11" s="1" t="s"/>
+      <x:c r="D11" s="1" t="s"/>
+      <x:c r="E11" s="1" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="1" t="s"/>
+      <x:c r="B12" s="1" t="s"/>
+      <x:c r="C12" s="1" t="s"/>
+      <x:c r="D12" s="1" t="s"/>
+      <x:c r="E12" s="1" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="A13" s="1" t="s"/>
+      <x:c r="B13" s="1" t="s"/>
+      <x:c r="C13" s="1" t="s"/>
+      <x:c r="D13" s="1" t="s"/>
+      <x:c r="E13" s="1" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="A14" s="1" t="s"/>
+      <x:c r="B14" s="1" t="s"/>
+      <x:c r="C14" s="1" t="s"/>
+      <x:c r="D14" s="1" t="s"/>
+      <x:c r="E14" s="1" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:dataValidations count="16">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1/>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Fixed data validation issue.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -527,7 +527,19 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -573,18 +585,6 @@
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1/>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1/>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1/>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -742,7 +742,19 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -788,18 +800,6 @@
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1/>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1/>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1/>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Copying a range now copies the data validations
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -10,6 +10,7 @@
     <x:sheet name="Validate Ranges" sheetId="3" r:id="rId3"/>
     <x:sheet name="Data Validation - Copy" sheetId="4" r:id="rId4"/>
     <x:sheet name="Validate Ranges - Copy" sheetId="5" r:id="rId5"/>
+    <x:sheet name="Copy From Range" sheetId="6" r:id="rId6"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="125725"/>
@@ -520,6 +521,7 @@
       <x:c r="C14" s="1" t="s"/>
       <x:c r="D14" s="1" t="s"/>
       <x:c r="E14" s="1" t="s"/>
+      <x:c r="G14" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:dataValidations count="16">
@@ -809,4 +811,246 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:G14"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="0" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:7">
+      <x:c r="A1" s="1" t="s"/>
+      <x:c r="B1" s="1" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:7">
+      <x:c r="A2" s="1" t="s"/>
+      <x:c r="B2" s="1" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:7">
+      <x:c r="B4" s="1" t="s"/>
+      <x:c r="C4" s="1" t="s"/>
+      <x:c r="D4" s="1" t="s"/>
+      <x:c r="F4" s="1" t="s"/>
+      <x:c r="G4" s="1" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:7">
+      <x:c r="B5" s="1" t="s"/>
+      <x:c r="C5" s="1" t="s"/>
+      <x:c r="D5" s="1" t="s"/>
+      <x:c r="F5" s="1" t="s"/>
+      <x:c r="G5" s="1" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:7">
+      <x:c r="B6" s="1" t="s"/>
+      <x:c r="C6" s="1" t="s"/>
+      <x:c r="D6" s="1" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:7">
+      <x:c r="B7" s="1" t="s"/>
+      <x:c r="C7" s="1" t="s"/>
+      <x:c r="D7" s="1" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:7">
+      <x:c r="A11" s="1" t="s"/>
+      <x:c r="B11" s="1" t="s"/>
+      <x:c r="C11" s="1" t="s"/>
+      <x:c r="D11" s="1" t="s"/>
+      <x:c r="E11" s="1" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:7">
+      <x:c r="A12" s="1" t="s"/>
+      <x:c r="B12" s="1" t="s"/>
+      <x:c r="C12" s="1" t="s"/>
+      <x:c r="D12" s="1" t="s"/>
+      <x:c r="E12" s="1" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:7">
+      <x:c r="A13" s="1" t="s"/>
+      <x:c r="B13" s="1" t="s"/>
+      <x:c r="C13" s="1" t="s"/>
+      <x:c r="D13" s="1" t="s"/>
+      <x:c r="E13" s="1" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:7">
+      <x:c r="A14" s="1" t="s"/>
+      <x:c r="B14" s="1" t="s"/>
+      <x:c r="C14" s="1" t="s"/>
+      <x:c r="D14" s="1" t="s"/>
+      <x:c r="E14" s="1" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:dataValidations count="40">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+  </x:dataValidations>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
cell.IsEmpty(includeFormats = true) now returns false if the cell has comments or data validations. It feels more natural that way. This also fixes copying ranges with validations.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -10,9 +10,12 @@
     <x:sheet name="Validate Ranges" sheetId="3" r:id="rId3"/>
     <x:sheet name="Data Validation - Copy" sheetId="4" r:id="rId4"/>
     <x:sheet name="Validate Ranges - Copy" sheetId="5" r:id="rId5"/>
-    <x:sheet name="Copy From Range" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Copy From Range 1" sheetId="6" r:id="rId6"/>
+    <x:sheet name="Copy From Range 2" sheetId="7" r:id="rId7"/>
   </x:sheets>
-  <x:definedNames/>
+  <x:definedNames>
+    <x:definedName name="YesNo">'Data Validation'!$C$1:$C$2</x:definedName>
+  </x:definedNames>
   <x:calcPr calcId="125725"/>
 </x:workbook>
 </file>
@@ -387,7 +390,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C5"/>
+  <x:dimension ref="A1:C6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -413,8 +416,12 @@
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s"/>
     </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s"/>
+      <x:c r="C6" s="0" t="s"/>
+    </x:row>
   </x:sheetData>
-  <x:dataValidations count="6">
+  <x:dataValidations count="7">
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -429,6 +436,10 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
       <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
+      <x:formula1>=YesNo</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
@@ -603,7 +614,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C5"/>
+  <x:dimension ref="A1:C6"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>
   </x:sheetViews>
@@ -629,8 +640,11 @@
     <x:row r="5" spans="1:3">
       <x:c r="A5" s="0" t="s"/>
     </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s"/>
+    </x:row>
   </x:sheetData>
-  <x:dataValidations count="6">
+  <x:dataValidations count="7">
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -645,6 +659,10 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
       <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
+      <x:formula1>=YesNo</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
@@ -818,6 +836,64 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
+  <x:dimension ref="A1:C6"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="0" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s"/>
+      <x:c r="C1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:3">
+      <x:c r="C2" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:3">
+      <x:c r="A4" s="0" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:3">
+      <x:c r="A5" s="0" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:3">
+      <x:c r="A6" s="0" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:dataValidations count="4">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2>5</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
+      <x:formula1>36526</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
+      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
+      <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+  </x:dataValidations>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
   <x:dimension ref="A1:G14"/>
   <x:sheetViews>
     <x:sheetView tabSelected="0" workbookViewId="0"/>

</xml_diff>

<commit_message>
Copying worksheets will copy the data validations with their relative targets
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -421,13 +421,29 @@
       <x:c r="C6" s="0" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="7">
+  <x:dataValidations count="9">
+    <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
     </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
-      <x:formula1>2</x:formula1>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C1:C1">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C2:C2">
+      <x:formula1/>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
@@ -440,14 +456,6 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
       <x:formula1>=YesNo</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -470,7 +478,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="7" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7">
@@ -535,8 +543,16 @@
       <x:c r="G14" s="0" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="16">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+  <x:dataValidations count="42">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B3">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B8:B10">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -544,7 +560,19 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -552,52 +580,136 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
-      <x:formula1>5</x:formula1>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
+      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -658,7 +770,7 @@
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula1>'Data Validation - Copy'!$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -863,10 +975,18 @@
       <x:c r="A6" s="0" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="4">
+  <x:dataValidations count="6">
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C1:C1">
+      <x:formula1/>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="none" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C2:C2">
+      <x:formula1/>
+      <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
       <x:formula1>36526</x:formula1>

</xml_diff>

<commit_message>
Data validations finally move when copying ranges/cells, inserting/deleting rows, etc.
</commit_message>
<xml_diff>
--- a/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML/ClosedXML/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -451,7 +451,7 @@
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula1>$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -770,7 +770,7 @@
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation - Copy'!$C$1:$C$2</x:formula1>
+      <x:formula1>$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
@@ -993,7 +993,7 @@
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula1>$C$1:$C$2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">

</xml_diff>